<commit_message>
Raw and Clean Data from SSA for June 20th and 21th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_tablero_oficial.xlsx
+++ b/data-validation/bitacora_historica_tablero_oficial.xlsx
@@ -395,467 +395,450 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2">
+    <row r="2" spans="1:6">
+      <c r="A2" s="2">
         <v>43983</v>
       </c>
+      <c r="B2">
+        <v>93435</v>
+      </c>
       <c r="C2">
-        <v>93435</v>
+        <v>150157</v>
       </c>
       <c r="D2">
-        <v>150157</v>
+        <v>38497</v>
       </c>
       <c r="E2">
-        <v>38497</v>
+        <v>10167</v>
       </c>
       <c r="F2">
-        <v>10167</v>
-      </c>
-      <c r="G2">
         <v>34.9</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2">
+    <row r="3" spans="1:6">
+      <c r="A3" s="2">
         <v>43984</v>
       </c>
+      <c r="B3">
+        <v>97326</v>
+      </c>
       <c r="C3">
-        <v>97326</v>
+        <v>153601</v>
       </c>
       <c r="D3">
-        <v>153601</v>
+        <v>42151</v>
       </c>
       <c r="E3">
-        <v>42151</v>
+        <v>10637</v>
       </c>
       <c r="F3">
-        <v>10637</v>
-      </c>
-      <c r="G3">
         <v>34.59</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2">
+    <row r="4" spans="1:6">
+      <c r="A4" s="2">
         <v>43985</v>
       </c>
+      <c r="B4">
+        <v>101238</v>
+      </c>
       <c r="C4">
-        <v>101238</v>
+        <v>157354</v>
       </c>
       <c r="D4">
-        <v>157354</v>
+        <v>44869</v>
       </c>
       <c r="E4">
-        <v>44869</v>
+        <v>11728</v>
       </c>
       <c r="F4">
-        <v>11728</v>
-      </c>
-      <c r="G4">
         <v>34.45</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" s="2">
+    <row r="5" spans="1:6">
+      <c r="A5" s="2">
         <v>43986</v>
       </c>
+      <c r="B5">
+        <v>105680</v>
+      </c>
       <c r="C5">
-        <v>105680</v>
+        <v>161724</v>
       </c>
       <c r="D5">
-        <v>161724</v>
+        <v>46659</v>
       </c>
       <c r="E5">
-        <v>46659</v>
+        <v>12545</v>
       </c>
       <c r="F5">
-        <v>12545</v>
-      </c>
-      <c r="G5">
         <v>34.24</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6" s="2">
+    <row r="6" spans="1:6">
+      <c r="A6" s="2">
         <v>43987</v>
       </c>
+      <c r="B6">
+        <v>110026</v>
+      </c>
       <c r="C6">
-        <v>110026</v>
+        <v>166049</v>
       </c>
       <c r="D6">
-        <v>166049</v>
+        <v>48822</v>
       </c>
       <c r="E6">
-        <v>48822</v>
+        <v>13170</v>
       </c>
       <c r="F6">
-        <v>13170</v>
-      </c>
-      <c r="G6">
         <v>34.03</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7" s="2">
+    <row r="7" spans="1:6">
+      <c r="A7" s="2">
         <v>43988</v>
       </c>
+      <c r="B7">
+        <v>113619</v>
+      </c>
       <c r="C7">
-        <v>113619</v>
+        <v>170434</v>
       </c>
       <c r="D7">
-        <v>170434</v>
+        <v>48273</v>
       </c>
       <c r="E7">
-        <v>48273</v>
+        <v>13511</v>
       </c>
       <c r="F7">
-        <v>13511</v>
-      </c>
-      <c r="G7">
         <v>33.72</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="1">
-        <v>6</v>
-      </c>
-      <c r="B8" s="2">
+    <row r="8" spans="1:6">
+      <c r="A8" s="2">
         <v>43989</v>
       </c>
+      <c r="B8">
+        <v>117103</v>
+      </c>
       <c r="C8">
-        <v>117103</v>
+        <v>173975</v>
       </c>
       <c r="D8">
-        <v>173975</v>
+        <v>45317</v>
       </c>
       <c r="E8">
-        <v>45317</v>
+        <v>13699</v>
       </c>
       <c r="F8">
-        <v>13699</v>
-      </c>
-      <c r="G8">
         <v>33.48</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="1">
-        <v>7</v>
-      </c>
-      <c r="B9" s="2">
+    <row r="9" spans="1:6">
+      <c r="A9" s="2">
         <v>43990</v>
       </c>
+      <c r="B9">
+        <v>120102</v>
+      </c>
       <c r="C9">
-        <v>120102</v>
+        <v>177875</v>
       </c>
       <c r="D9">
-        <v>177875</v>
+        <v>46398</v>
       </c>
       <c r="E9">
-        <v>46398</v>
+        <v>14053</v>
       </c>
       <c r="F9">
-        <v>14053</v>
-      </c>
-      <c r="G9">
         <v>33.32</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="1">
-        <v>8</v>
-      </c>
-      <c r="B10" s="2">
+    <row r="10" spans="1:6">
+      <c r="A10" s="2">
         <v>43991</v>
       </c>
+      <c r="B10">
+        <v>124301</v>
+      </c>
       <c r="C10">
-        <v>124301</v>
+        <v>182077</v>
       </c>
       <c r="D10">
-        <v>182077</v>
+        <v>50677</v>
       </c>
       <c r="E10">
-        <v>50677</v>
+        <v>14649</v>
       </c>
       <c r="F10">
-        <v>14649</v>
-      </c>
-      <c r="G10">
         <v>33.21</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="1">
-        <v>9</v>
-      </c>
-      <c r="B11" s="2">
+    <row r="11" spans="1:6">
+      <c r="A11" s="2">
         <v>43992</v>
       </c>
+      <c r="B11">
+        <v>129184</v>
+      </c>
       <c r="C11">
-        <v>129184</v>
+        <v>186570</v>
       </c>
       <c r="D11">
-        <v>186570</v>
+        <v>53608</v>
       </c>
       <c r="E11">
-        <v>53608</v>
+        <v>15357</v>
       </c>
       <c r="F11">
-        <v>15357</v>
-      </c>
-      <c r="G11">
         <v>33.11</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="1">
-        <v>10</v>
-      </c>
-      <c r="B12" s="2">
+    <row r="12" spans="1:6">
+      <c r="A12" s="2">
         <v>43993</v>
       </c>
+      <c r="B12">
+        <v>133974</v>
+      </c>
       <c r="C12">
-        <v>133974</v>
+        <v>191465</v>
       </c>
       <c r="D12">
-        <v>191465</v>
+        <v>55700</v>
       </c>
       <c r="E12">
-        <v>55700</v>
+        <v>15944</v>
       </c>
       <c r="F12">
-        <v>15944</v>
-      </c>
-      <c r="G12">
         <v>33.01</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="1">
-        <v>11</v>
-      </c>
-      <c r="B13" s="2">
+    <row r="13" spans="1:6">
+      <c r="A13" s="2">
         <v>43994</v>
       </c>
+      <c r="B13">
+        <v>139196</v>
+      </c>
       <c r="C13">
-        <v>139196</v>
+        <v>197590</v>
       </c>
       <c r="D13">
-        <v>197590</v>
+        <v>56928</v>
       </c>
       <c r="E13">
-        <v>56928</v>
+        <v>16448</v>
       </c>
       <c r="F13">
-        <v>16448</v>
-      </c>
-      <c r="G13">
         <v>32.78</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="1">
-        <v>12</v>
-      </c>
-      <c r="B14" s="2">
+    <row r="14" spans="1:6">
+      <c r="A14" s="2">
         <v>43995</v>
       </c>
+      <c r="B14">
+        <v>142690</v>
+      </c>
       <c r="C14">
-        <v>142690</v>
+        <v>202139</v>
       </c>
       <c r="D14">
-        <v>202139</v>
+        <v>56926</v>
       </c>
       <c r="E14">
-        <v>56926</v>
+        <v>16872</v>
       </c>
       <c r="F14">
-        <v>16872</v>
-      </c>
-      <c r="G14">
         <v>32.66</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="1">
-        <v>13</v>
-      </c>
-      <c r="B15" s="2">
+    <row r="15" spans="1:6">
+      <c r="A15" s="2">
         <v>43996</v>
       </c>
+      <c r="B15">
+        <v>146837</v>
+      </c>
       <c r="C15">
-        <v>146837</v>
+        <v>207076</v>
       </c>
       <c r="D15">
-        <v>207076</v>
+        <v>52636</v>
       </c>
       <c r="E15">
-        <v>52636</v>
+        <v>17141</v>
       </c>
       <c r="F15">
-        <v>17141</v>
-      </c>
-      <c r="G15">
         <v>32.5</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="1">
-        <v>14</v>
-      </c>
-      <c r="B16" s="2">
+    <row r="16" spans="1:6">
+      <c r="A16" s="2">
         <v>43997</v>
       </c>
+      <c r="B16">
+        <v>150264</v>
+      </c>
       <c r="C16">
-        <v>150264</v>
+        <v>211616</v>
       </c>
       <c r="D16">
-        <v>211616</v>
+        <v>53217</v>
       </c>
       <c r="E16">
-        <v>53217</v>
+        <v>17580</v>
       </c>
       <c r="F16">
-        <v>17580</v>
-      </c>
-      <c r="G16">
         <v>32.36</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="1">
-        <v>15</v>
-      </c>
-      <c r="B17" s="2">
+    <row r="17" spans="1:6">
+      <c r="A17" s="2">
         <v>43998</v>
       </c>
+      <c r="B17">
+        <v>154863</v>
+      </c>
       <c r="C17">
-        <v>154863</v>
+        <v>216857</v>
       </c>
       <c r="D17">
-        <v>216857</v>
+        <v>56843</v>
       </c>
       <c r="E17">
-        <v>56843</v>
+        <v>18310</v>
       </c>
       <c r="F17">
-        <v>18310</v>
-      </c>
-      <c r="G17">
         <v>32.29</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="1">
-        <v>16</v>
-      </c>
-      <c r="B18" s="2">
+    <row r="18" spans="1:6">
+      <c r="A18" s="2">
         <v>43999</v>
       </c>
+      <c r="B18">
+        <v>159793</v>
+      </c>
       <c r="C18">
-        <v>159793</v>
+        <v>222801</v>
       </c>
       <c r="D18">
-        <v>222801</v>
+        <v>59076</v>
       </c>
       <c r="E18">
-        <v>59076</v>
+        <v>19080</v>
       </c>
       <c r="F18">
-        <v>19080</v>
-      </c>
-      <c r="G18">
         <v>32.06</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="1">
-        <v>17</v>
-      </c>
-      <c r="B19" s="2">
+    <row r="19" spans="1:6">
+      <c r="A19" s="2">
         <v>44000</v>
       </c>
+      <c r="B19">
+        <v>165455</v>
+      </c>
       <c r="C19">
-        <v>165455</v>
+        <v>228248</v>
       </c>
       <c r="D19">
-        <v>228248</v>
+        <v>59778</v>
       </c>
       <c r="E19">
-        <v>59778</v>
+        <v>19747</v>
       </c>
       <c r="F19">
-        <v>19747</v>
-      </c>
-      <c r="G19">
         <v>31.86</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="1">
-        <v>18</v>
-      </c>
-      <c r="B20" s="3">
+    <row r="20" spans="1:6">
+      <c r="A20" s="2">
         <v>44001</v>
       </c>
+      <c r="B20">
+        <v>170485</v>
+      </c>
       <c r="C20">
-        <v>170485</v>
+        <v>233137</v>
       </c>
       <c r="D20">
-        <v>233137</v>
+        <v>62245</v>
       </c>
       <c r="E20">
-        <v>62245</v>
+        <v>20394</v>
       </c>
       <c r="F20">
-        <v>20394</v>
-      </c>
-      <c r="G20">
         <v>31.72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="2">
+        <v>44002</v>
+      </c>
+      <c r="B21">
+        <v>175202</v>
+      </c>
+      <c r="C21">
+        <v>238129</v>
+      </c>
+      <c r="D21">
+        <v>60621</v>
+      </c>
+      <c r="E21">
+        <v>20781</v>
+      </c>
+      <c r="F21">
+        <v>31.46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="3">
+        <v>44003</v>
+      </c>
+      <c r="B22">
+        <v>180545</v>
+      </c>
+      <c r="C22">
+        <v>242393</v>
+      </c>
+      <c r="D22">
+        <v>56590</v>
+      </c>
+      <c r="E22">
+        <v>21825</v>
+      </c>
+      <c r="F22">
+        <v>31.61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Raw and Clean Data from SSSA for October 7, 8
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_tablero_oficial.xlsx
+++ b/data-validation/bitacora_historica_tablero_oficial.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/PADeCI/covid19-mx-data/data-validation/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F8760A5-04FC-3549-9656-2CF336295FF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="130">
   <si>
     <t>Fecha</t>
   </si>
@@ -400,14 +406,17 @@
     <t>2020-09-30</t>
   </si>
   <si>
-    <t>2020-10-05</t>
+    <t>2020-09-31</t>
+  </si>
+  <si>
+    <t>2020-10-08</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -419,6 +428,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -459,22 +474,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -516,7 +540,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -548,9 +572,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -582,6 +624,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -757,14 +817,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F124"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F132"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
+      <selection activeCell="A125" sqref="A125"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -784,7 +849,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -804,7 +869,7 @@
         <v>34.9</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -821,10 +886,10 @@
         <v>10637</v>
       </c>
       <c r="F3">
-        <v>34.59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>34.590000000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -841,10 +906,10 @@
         <v>11728</v>
       </c>
       <c r="F4">
-        <v>34.45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>34.450000000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -864,7 +929,7 @@
         <v>34.24</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -884,7 +949,7 @@
         <v>34.03</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -904,7 +969,7 @@
         <v>33.72</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -921,10 +986,10 @@
         <v>13699</v>
       </c>
       <c r="F8">
-        <v>33.48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>33.479999999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -944,7 +1009,7 @@
         <v>33.32</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -964,7 +1029,7 @@
         <v>33.21</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -984,7 +1049,7 @@
         <v>33.11</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1004,7 +1069,7 @@
         <v>33.01</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1024,7 +1089,7 @@
         <v>32.78</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -1041,10 +1106,10 @@
         <v>16872</v>
       </c>
       <c r="F14">
-        <v>32.66</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+        <v>32.659999999999997</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -1064,7 +1129,7 @@
         <v>32.5</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -1084,7 +1149,7 @@
         <v>32.36</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -1104,7 +1169,7 @@
         <v>32.29</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -1124,7 +1189,7 @@
         <v>32.06</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -1144,7 +1209,7 @@
         <v>31.86</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -1164,7 +1229,7 @@
         <v>31.72</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -1184,7 +1249,7 @@
         <v>31.46</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -1204,7 +1269,7 @@
         <v>31.61</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -1224,7 +1289,7 @@
         <v>31.69</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>28</v>
       </c>
@@ -1244,7 +1309,7 @@
         <v>31.6</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -1264,7 +1329,7 @@
         <v>31.58</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -1284,7 +1349,7 @@
         <v>31.46</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -1304,7 +1369,7 @@
         <v>31.37</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -1324,7 +1389,7 @@
         <v>31.24</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>33</v>
       </c>
@@ -1344,7 +1409,7 @@
         <v>31.11</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>34</v>
       </c>
@@ -1364,7 +1429,7 @@
         <v>30.95</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>35</v>
       </c>
@@ -1384,7 +1449,7 @@
         <v>30.78</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>36</v>
       </c>
@@ -1404,7 +1469,7 @@
         <v>30.73</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>37</v>
       </c>
@@ -1424,7 +1489,7 @@
         <v>30.52</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>38</v>
       </c>
@@ -1444,7 +1509,7 @@
         <v>30.35</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>39</v>
       </c>
@@ -1464,7 +1529,7 @@
         <v>30.18</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>40</v>
       </c>
@@ -1484,7 +1549,7 @@
         <v>30.02</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>41</v>
       </c>
@@ -1504,7 +1569,7 @@
         <v>29.94</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>42</v>
       </c>
@@ -1524,7 +1589,7 @@
         <v>29.89</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>43</v>
       </c>
@@ -1544,7 +1609,7 @@
         <v>29.78</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>44</v>
       </c>
@@ -1564,7 +1629,7 @@
         <v>29.67</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>45</v>
       </c>
@@ -1584,7 +1649,7 @@
         <v>29.5</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>46</v>
       </c>
@@ -1604,7 +1669,7 @@
         <v>29.33</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>47</v>
       </c>
@@ -1624,7 +1689,7 @@
         <v>29.25</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>48</v>
       </c>
@@ -1644,7 +1709,7 @@
         <v>29.21</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>49</v>
       </c>
@@ -1664,7 +1729,7 @@
         <v>29.12</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>50</v>
       </c>
@@ -1684,7 +1749,7 @@
         <v>29.05</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>51</v>
       </c>
@@ -1704,7 +1769,7 @@
         <v>28.95</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>52</v>
       </c>
@@ -1724,7 +1789,7 @@
         <v>28.81</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>53</v>
       </c>
@@ -1744,7 +1809,7 @@
         <v>28.66</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>54</v>
       </c>
@@ -1764,7 +1829,7 @@
         <v>28.55</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>55</v>
       </c>
@@ -1784,7 +1849,7 @@
         <v>28.43</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>56</v>
       </c>
@@ -1804,7 +1869,7 @@
         <v>28.33</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>57</v>
       </c>
@@ -1824,7 +1889,7 @@
         <v>28.24</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>58</v>
       </c>
@@ -1844,7 +1909,7 @@
         <v>28.12</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>59</v>
       </c>
@@ -1864,7 +1929,7 @@
         <v>27.97</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>60</v>
       </c>
@@ -1884,7 +1949,7 @@
         <v>27.89</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>61</v>
       </c>
@@ -1904,7 +1969,7 @@
         <v>27.78</v>
       </c>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>62</v>
       </c>
@@ -1924,7 +1989,7 @@
         <v>27.72</v>
       </c>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>63</v>
       </c>
@@ -1944,7 +2009,7 @@
         <v>27.63</v>
       </c>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>64</v>
       </c>
@@ -1964,7 +2029,7 @@
         <v>27.52</v>
       </c>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>65</v>
       </c>
@@ -1984,7 +2049,7 @@
         <v>27.38</v>
       </c>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>66</v>
       </c>
@@ -2004,7 +2069,7 @@
         <v>27.16</v>
       </c>
     </row>
-    <row r="63" spans="1:6">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>67</v>
       </c>
@@ -2024,7 +2089,7 @@
         <v>27.02</v>
       </c>
     </row>
-    <row r="64" spans="1:6">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>68</v>
       </c>
@@ -2044,7 +2109,7 @@
         <v>26.92</v>
       </c>
     </row>
-    <row r="65" spans="1:6">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>69</v>
       </c>
@@ -2064,7 +2129,7 @@
         <v>26.88</v>
       </c>
     </row>
-    <row r="66" spans="1:6">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>70</v>
       </c>
@@ -2084,7 +2149,7 @@
         <v>26.86</v>
       </c>
     </row>
-    <row r="67" spans="1:6">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>71</v>
       </c>
@@ -2104,7 +2169,7 @@
         <v>26.83</v>
       </c>
     </row>
-    <row r="68" spans="1:6">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>72</v>
       </c>
@@ -2124,7 +2189,7 @@
         <v>26.8</v>
       </c>
     </row>
-    <row r="69" spans="1:6">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>73</v>
       </c>
@@ -2144,7 +2209,7 @@
         <v>26.74</v>
       </c>
     </row>
-    <row r="70" spans="1:6">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>74</v>
       </c>
@@ -2164,7 +2229,7 @@
         <v>26.67</v>
       </c>
     </row>
-    <row r="71" spans="1:6">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>75</v>
       </c>
@@ -2184,7 +2249,7 @@
         <v>26.61</v>
       </c>
     </row>
-    <row r="72" spans="1:6">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>76</v>
       </c>
@@ -2204,7 +2269,7 @@
         <v>26.56</v>
       </c>
     </row>
-    <row r="73" spans="1:6">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>77</v>
       </c>
@@ -2224,7 +2289,7 @@
         <v>26.51</v>
       </c>
     </row>
-    <row r="74" spans="1:6">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>78</v>
       </c>
@@ -2244,7 +2309,7 @@
         <v>26.49</v>
       </c>
     </row>
-    <row r="75" spans="1:6">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>79</v>
       </c>
@@ -2264,7 +2329,7 @@
         <v>26.39</v>
       </c>
     </row>
-    <row r="76" spans="1:6">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>80</v>
       </c>
@@ -2284,7 +2349,7 @@
         <v>26.33</v>
       </c>
     </row>
-    <row r="77" spans="1:6">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>81</v>
       </c>
@@ -2304,7 +2369,7 @@
         <v>26.25</v>
       </c>
     </row>
-    <row r="78" spans="1:6">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>82</v>
       </c>
@@ -2324,7 +2389,7 @@
         <v>26.21</v>
       </c>
     </row>
-    <row r="79" spans="1:6">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>83</v>
       </c>
@@ -2344,7 +2409,7 @@
         <v>26.17</v>
       </c>
     </row>
-    <row r="80" spans="1:6">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>84</v>
       </c>
@@ -2364,7 +2429,7 @@
         <v>26.15</v>
       </c>
     </row>
-    <row r="81" spans="1:6">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>85</v>
       </c>
@@ -2384,7 +2449,7 @@
         <v>26.09</v>
       </c>
     </row>
-    <row r="82" spans="1:6">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>86</v>
       </c>
@@ -2404,7 +2469,7 @@
         <v>26.02</v>
       </c>
     </row>
-    <row r="83" spans="1:6">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>87</v>
       </c>
@@ -2424,7 +2489,7 @@
         <v>25.9</v>
       </c>
     </row>
-    <row r="84" spans="1:6">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>88</v>
       </c>
@@ -2444,7 +2509,7 @@
         <v>25.86</v>
       </c>
     </row>
-    <row r="85" spans="1:6">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>89</v>
       </c>
@@ -2464,7 +2529,7 @@
         <v>25.81</v>
       </c>
     </row>
-    <row r="86" spans="1:6">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>90</v>
       </c>
@@ -2484,7 +2549,7 @@
         <v>25.81</v>
       </c>
     </row>
-    <row r="87" spans="1:6">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>91</v>
       </c>
@@ -2504,7 +2569,7 @@
         <v>25.76</v>
       </c>
     </row>
-    <row r="88" spans="1:6">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>92</v>
       </c>
@@ -2524,7 +2589,7 @@
         <v>25.7</v>
       </c>
     </row>
-    <row r="89" spans="1:6">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>93</v>
       </c>
@@ -2544,7 +2609,7 @@
         <v>25.64</v>
       </c>
     </row>
-    <row r="90" spans="1:6">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>94</v>
       </c>
@@ -2564,7 +2629,7 @@
         <v>25.57</v>
       </c>
     </row>
-    <row r="91" spans="1:6">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>95</v>
       </c>
@@ -2584,7 +2649,7 @@
         <v>25.50328538207777</v>
       </c>
     </row>
-    <row r="92" spans="1:6">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>96</v>
       </c>
@@ -2604,7 +2669,7 @@
         <v>25.46</v>
       </c>
     </row>
-    <row r="93" spans="1:6">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>97</v>
       </c>
@@ -2624,7 +2689,7 @@
         <v>25.42</v>
       </c>
     </row>
-    <row r="94" spans="1:6">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>98</v>
       </c>
@@ -2644,7 +2709,7 @@
         <v>25.36</v>
       </c>
     </row>
-    <row r="95" spans="1:6">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>99</v>
       </c>
@@ -2664,7 +2729,7 @@
         <v>25.32</v>
       </c>
     </row>
-    <row r="96" spans="1:6">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>100</v>
       </c>
@@ -2684,7 +2749,7 @@
         <v>25.25</v>
       </c>
     </row>
-    <row r="97" spans="1:6">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>101</v>
       </c>
@@ -2704,7 +2769,7 @@
         <v>25.17</v>
       </c>
     </row>
-    <row r="98" spans="1:6">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>102</v>
       </c>
@@ -2724,7 +2789,7 @@
         <v>25.06</v>
       </c>
     </row>
-    <row r="99" spans="1:6">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>103</v>
       </c>
@@ -2744,7 +2809,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="100" spans="1:6">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>104</v>
       </c>
@@ -2764,7 +2829,7 @@
         <v>24.98</v>
       </c>
     </row>
-    <row r="101" spans="1:6">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>105</v>
       </c>
@@ -2784,7 +2849,7 @@
         <v>24.93</v>
       </c>
     </row>
-    <row r="102" spans="1:6">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>106</v>
       </c>
@@ -2804,7 +2869,7 @@
         <v>24.88</v>
       </c>
     </row>
-    <row r="103" spans="1:6">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>107</v>
       </c>
@@ -2824,7 +2889,7 @@
         <v>24.81</v>
       </c>
     </row>
-    <row r="104" spans="1:6">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>108</v>
       </c>
@@ -2844,7 +2909,7 @@
         <v>24.73</v>
       </c>
     </row>
-    <row r="105" spans="1:6">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>109</v>
       </c>
@@ -2864,7 +2929,7 @@
         <v>24.67</v>
       </c>
     </row>
-    <row r="106" spans="1:6">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>110</v>
       </c>
@@ -2884,7 +2949,7 @@
         <v>24.59</v>
       </c>
     </row>
-    <row r="107" spans="1:6">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>111</v>
       </c>
@@ -2904,7 +2969,7 @@
         <v>24.57</v>
       </c>
     </row>
-    <row r="108" spans="1:6">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>112</v>
       </c>
@@ -2924,7 +2989,7 @@
         <v>24.55</v>
       </c>
     </row>
-    <row r="109" spans="1:6">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>113</v>
       </c>
@@ -2944,7 +3009,7 @@
         <v>24.5</v>
       </c>
     </row>
-    <row r="110" spans="1:6">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>114</v>
       </c>
@@ -2964,7 +3029,7 @@
         <v>24.48</v>
       </c>
     </row>
-    <row r="111" spans="1:6">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>115</v>
       </c>
@@ -2984,7 +3049,7 @@
         <v>24.44</v>
       </c>
     </row>
-    <row r="112" spans="1:6">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>116</v>
       </c>
@@ -3004,7 +3069,7 @@
         <v>24.39</v>
       </c>
     </row>
-    <row r="113" spans="1:6">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>117</v>
       </c>
@@ -3024,7 +3089,7 @@
         <v>24.39</v>
       </c>
     </row>
-    <row r="114" spans="1:6">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>118</v>
       </c>
@@ -3044,7 +3109,7 @@
         <v>24.35</v>
       </c>
     </row>
-    <row r="115" spans="1:6">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>119</v>
       </c>
@@ -3064,7 +3129,7 @@
         <v>24.32</v>
       </c>
     </row>
-    <row r="116" spans="1:6">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>120</v>
       </c>
@@ -3084,7 +3149,7 @@
         <v>24.28</v>
       </c>
     </row>
-    <row r="117" spans="1:6">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>121</v>
       </c>
@@ -3104,7 +3169,7 @@
         <v>24.22</v>
       </c>
     </row>
-    <row r="118" spans="1:6">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>122</v>
       </c>
@@ -3124,7 +3189,7 @@
         <v>24.16</v>
       </c>
     </row>
-    <row r="119" spans="1:6">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>123</v>
       </c>
@@ -3144,7 +3209,7 @@
         <v>24.09</v>
       </c>
     </row>
-    <row r="120" spans="1:6">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>124</v>
       </c>
@@ -3164,7 +3229,7 @@
         <v>24.03</v>
       </c>
     </row>
-    <row r="121" spans="1:6">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>125</v>
       </c>
@@ -3184,7 +3249,7 @@
         <v>24.01</v>
       </c>
     </row>
-    <row r="122" spans="1:6">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>126</v>
       </c>
@@ -3204,7 +3269,7 @@
         <v>23.99</v>
       </c>
     </row>
-    <row r="123" spans="1:6">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>127</v>
       </c>
@@ -3224,27 +3289,188 @@
         <v>23.94</v>
       </c>
     </row>
-    <row r="124" spans="1:6">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>128</v>
       </c>
       <c r="B124">
+        <v>748315</v>
+      </c>
+      <c r="C124">
+        <v>884896</v>
+      </c>
+      <c r="D124">
+        <v>88659</v>
+      </c>
+      <c r="E124">
+        <v>78078</v>
+      </c>
+      <c r="F124">
+        <v>23.88</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A125" s="2">
+        <v>44105</v>
+      </c>
+      <c r="B125">
+        <v>748315</v>
+      </c>
+      <c r="C125">
+        <v>884896</v>
+      </c>
+      <c r="D125">
+        <v>88659</v>
+      </c>
+      <c r="E125">
+        <v>78078</v>
+      </c>
+      <c r="F125">
+        <v>23.88031778061378</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A126" s="2">
+        <v>44106</v>
+      </c>
+      <c r="B126">
+        <v>753090</v>
+      </c>
+      <c r="C126">
+        <v>893324</v>
+      </c>
+      <c r="D126">
+        <v>89183</v>
+      </c>
+      <c r="E126">
+        <v>78492</v>
+      </c>
+      <c r="F126">
+        <v>23.810832702598631</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A127" s="2">
+        <v>44107</v>
+      </c>
+      <c r="B127">
+        <v>757953</v>
+      </c>
+      <c r="C127">
+        <v>901110</v>
+      </c>
+      <c r="D127">
+        <v>90194</v>
+      </c>
+      <c r="E127">
+        <v>78880</v>
+      </c>
+      <c r="F127">
+        <v>23.7492298335121</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A128" s="2">
+        <v>44108</v>
+      </c>
+      <c r="B128">
+        <v>761665</v>
+      </c>
+      <c r="C128">
+        <v>907331</v>
+      </c>
+      <c r="D128">
+        <v>85743</v>
+      </c>
+      <c r="E128">
+        <v>79088</v>
+      </c>
+      <c r="F128">
+        <v>23.707535465066659</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A129" s="2">
+        <v>44109</v>
+      </c>
+      <c r="B129">
         <v>765082</v>
       </c>
-      <c r="C124">
+      <c r="C129">
         <v>913155</v>
       </c>
-      <c r="D124">
+      <c r="D129">
         <v>80345</v>
       </c>
-      <c r="E124">
+      <c r="E129">
         <v>79268</v>
       </c>
-      <c r="F124">
-        <v>23.68</v>
+      <c r="F129">
+        <v>23.675501449517832</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A130" s="2">
+        <v>44110</v>
+      </c>
+      <c r="B130">
+        <v>769558</v>
+      </c>
+      <c r="C130">
+        <v>933316</v>
+      </c>
+      <c r="D130">
+        <v>32797</v>
+      </c>
+      <c r="E130">
+        <v>79714</v>
+      </c>
+      <c r="F130">
+        <v>23.652018431359298</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A131" s="2">
+        <v>44111</v>
+      </c>
+      <c r="B131">
+        <v>774020</v>
+      </c>
+      <c r="C131">
+        <v>940994</v>
+      </c>
+      <c r="D131">
+        <v>36802</v>
+      </c>
+      <c r="E131">
+        <v>80083</v>
+      </c>
+      <c r="F131">
+        <v>23.618123562698639</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>129</v>
+      </c>
+      <c r="B132">
+        <v>804488</v>
+      </c>
+      <c r="C132">
+        <v>948928</v>
+      </c>
+      <c r="D132">
+        <v>299866</v>
+      </c>
+      <c r="E132">
+        <v>83096</v>
+      </c>
+      <c r="F132">
+        <v>23.5</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Raw and Clean Data from SSA for December 7
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_tablero_oficial.xlsx
+++ b/data-validation/bitacora_historica_tablero_oficial.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="142">
   <si>
     <t>Fecha</t>
   </si>
@@ -437,6 +437,9 @@
   </si>
   <si>
     <t>2020-10-27</t>
+  </si>
+  <si>
+    <t>2020-12-07</t>
   </si>
 </sst>
 </file>
@@ -798,7 +801,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F151"/>
+  <dimension ref="A1:F152"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -3824,6 +3827,26 @@
         <v>22.85</v>
       </c>
     </row>
+    <row r="152" spans="1:6">
+      <c r="A152" t="s">
+        <v>141</v>
+      </c>
+      <c r="B152">
+        <v>1182249</v>
+      </c>
+      <c r="C152">
+        <v>1456073</v>
+      </c>
+      <c r="D152">
+        <v>384905</v>
+      </c>
+      <c r="E152">
+        <v>110074</v>
+      </c>
+      <c r="F152">
+        <v>21.13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>